<commit_message>
jkzl - auto verify yzm
</commit_message>
<xml_diff>
--- a/miaoTemp/武汉/楚天/汉阳用户.xlsx
+++ b/miaoTemp/武汉/楚天/汉阳用户.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSharp\DotnetMiao\miaoTemp\武汉\楚天\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CA9ADB-99A7-4F71-9819-CF5A9BB77B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA931231-5EB1-4B37-94D5-E0BB7FA65D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2220" yWindow="1200" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="汉阳" sheetId="1" r:id="rId1"/>
     <sheet name="汉阳成功" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -680,7 +679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C7:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
@@ -1087,7 +1086,9 @@
       <c r="D41" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E41" s="7"/>
+      <c r="E41" s="7">
+        <v>17152022762</v>
+      </c>
       <c r="F41" s="7">
         <v>18171438859</v>
       </c>

</xml_diff>